<commit_message>
push for normal distribution method
</commit_message>
<xml_diff>
--- a/TQQQ_X_test_oot.xlsx
+++ b/TQQQ_X_test_oot.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3486,6 +3486,278 @@
         <v>-0.1109024416122099</v>
       </c>
     </row>
+    <row r="183" spans="1:5">
+      <c r="A183">
+        <v>82.3517499923706</v>
+      </c>
+      <c r="B183">
+        <v>75.71989986419678</v>
+      </c>
+      <c r="C183">
+        <v>42.23194306946534</v>
+      </c>
+      <c r="D183">
+        <v>4.88114871383457</v>
+      </c>
+      <c r="E183">
+        <v>0.003224937955573992</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184">
+        <v>82.47575016021729</v>
+      </c>
+      <c r="B184">
+        <v>75.82839992523193</v>
+      </c>
+      <c r="C184">
+        <v>36.63498098307812</v>
+      </c>
+      <c r="D184">
+        <v>4.257566297211689</v>
+      </c>
+      <c r="E184">
+        <v>-0.01797219810061368</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185">
+        <v>82.66000022888184</v>
+      </c>
+      <c r="B185">
+        <v>75.95449993133545</v>
+      </c>
+      <c r="C185">
+        <v>41.94715559232957</v>
+      </c>
+      <c r="D185">
+        <v>3.568726936736319</v>
+      </c>
+      <c r="E185">
+        <v>0.0821293428115375</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186">
+        <v>82.84075012207032</v>
+      </c>
+      <c r="B186">
+        <v>76.11509990692139</v>
+      </c>
+      <c r="C186">
+        <v>52.60227175983852</v>
+      </c>
+      <c r="D186">
+        <v>3.626715821975181</v>
+      </c>
+      <c r="E186">
+        <v>0.1116664211506126</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187">
+        <v>83.10575027465821</v>
+      </c>
+      <c r="B187">
+        <v>76.30269992828369</v>
+      </c>
+      <c r="C187">
+        <v>57.03749658271517</v>
+      </c>
+      <c r="D187">
+        <v>3.864082544896479</v>
+      </c>
+      <c r="E187">
+        <v>0.1589229220701076</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188">
+        <v>83.36525020599365</v>
+      </c>
+      <c r="B188">
+        <v>76.51909992218017</v>
+      </c>
+      <c r="C188">
+        <v>55.61904685014895</v>
+      </c>
+      <c r="D188">
+        <v>4.107682368461616</v>
+      </c>
+      <c r="E188">
+        <v>0.09223540229728933</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189">
+        <v>83.57775020599365</v>
+      </c>
+      <c r="B189">
+        <v>76.72309993743896</v>
+      </c>
+      <c r="C189">
+        <v>51.80517312587544</v>
+      </c>
+      <c r="D189">
+        <v>4.183193892801236</v>
+      </c>
+      <c r="E189">
+        <v>0.09491349645901925</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190">
+        <v>83.59100017547607</v>
+      </c>
+      <c r="B190">
+        <v>76.82839992523193</v>
+      </c>
+      <c r="C190">
+        <v>40.8894915209647</v>
+      </c>
+      <c r="D190">
+        <v>3.992264812935886</v>
+      </c>
+      <c r="E190">
+        <v>-0.04811161930917729</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191">
+        <v>83.66150016784668</v>
+      </c>
+      <c r="B191">
+        <v>77.03139995574951</v>
+      </c>
+      <c r="C191">
+        <v>44.84915308212367</v>
+      </c>
+      <c r="D191">
+        <v>3.71485632323183</v>
+      </c>
+      <c r="E191">
+        <v>-0.02212488395006229</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192">
+        <v>83.76750011444092</v>
+      </c>
+      <c r="B192">
+        <v>77.23459995269775</v>
+      </c>
+      <c r="C192">
+        <v>47.54289676063065</v>
+      </c>
+      <c r="D192">
+        <v>3.650751689194498</v>
+      </c>
+      <c r="E192">
+        <v>-0.0644647319519206</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193">
+        <v>83.84950008392335</v>
+      </c>
+      <c r="B193">
+        <v>77.44609992980958</v>
+      </c>
+      <c r="C193">
+        <v>51.95256264927125</v>
+      </c>
+      <c r="D193">
+        <v>3.667516880191039</v>
+      </c>
+      <c r="E193">
+        <v>-0.05852386668854559</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194">
+        <v>83.85550003051758</v>
+      </c>
+      <c r="B194">
+        <v>77.70339992523193</v>
+      </c>
+      <c r="C194">
+        <v>53.80055688312157</v>
+      </c>
+      <c r="D194">
+        <v>3.625168273640944</v>
+      </c>
+      <c r="E194">
+        <v>-0.04645531734059793</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195">
+        <v>83.79325008392334</v>
+      </c>
+      <c r="B195">
+        <v>77.91949993133545</v>
+      </c>
+      <c r="C195">
+        <v>52.14447479190592</v>
+      </c>
+      <c r="D195">
+        <v>3.557500373388179</v>
+      </c>
+      <c r="E195">
+        <v>0.01996464295223821</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196">
+        <v>83.72825012207031</v>
+      </c>
+      <c r="B196">
+        <v>78.14899993896485</v>
+      </c>
+      <c r="C196">
+        <v>51.30507497649368</v>
+      </c>
+      <c r="D196">
+        <v>3.576998871603226</v>
+      </c>
+      <c r="E196">
+        <v>0.01209921332774422</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197">
+        <v>83.70825004577637</v>
+      </c>
+      <c r="B197">
+        <v>78.35069992065429</v>
+      </c>
+      <c r="C197">
+        <v>49.49100980073005</v>
+      </c>
+      <c r="D197">
+        <v>3.556276933230153</v>
+      </c>
+      <c r="E197">
+        <v>0.03165325655515838</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198">
+        <v>83.66500015258789</v>
+      </c>
+      <c r="B198">
+        <v>78.54599990844727</v>
+      </c>
+      <c r="C198">
+        <v>56.28938443481556</v>
+      </c>
+      <c r="D198">
+        <v>3.651115444205833</v>
+      </c>
+      <c r="E198">
+        <v>0.03414697643152742</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>